<commit_message>
UPdated Login sheet and DataRetrival
</commit_message>
<xml_diff>
--- a/dataSheet/Login.xlsx
+++ b/dataSheet/Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10613203\Desktop\selne\dccmWorkspace\dccm\dataSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10637217\Desktop\DCCM\Workspace\LearnProject\dataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F012D075-BAAE-4F9A-ABC5-AB769004AFC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE8FF25-6A1A-49A9-9A72-8B7BFA8D1CFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="624" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,43 +24,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>sno</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>UserID</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>TestCaseDescription</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Release@321</t>
   </si>
   <si>
-    <t>https://dccm-preuat.fst.lntinfotech.com</t>
-  </si>
-  <si>
     <t>automationtwo</t>
   </si>
   <si>
-    <t>automationone</t>
+    <t>Exec_Flag</t>
+  </si>
+  <si>
+    <t>BPC_Flag</t>
+  </si>
+  <si>
+    <t>IVRINQ_AccountNumber</t>
+  </si>
+  <si>
+    <t>Account_Type_Code</t>
+  </si>
+  <si>
+    <t>INGLST_SearchInvestmentCode</t>
+  </si>
+  <si>
+    <t>MUSCH_ScreenCode</t>
+  </si>
+  <si>
+    <t>Actual_Free_Units</t>
+  </si>
+  <si>
+    <t>Expected_Free_Units</t>
+  </si>
+  <si>
+    <t>Actual_DSC</t>
+  </si>
+  <si>
+    <t>Expected_DSC</t>
+  </si>
+  <si>
+    <t>ActualErrorMessage</t>
+  </si>
+  <si>
+    <t>ExpectedErrorMessage</t>
+  </si>
+  <si>
+    <t>TC_Result</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +221,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="25">
     <fill>
@@ -317,7 +364,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,21 +546,24 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -895,63 +945,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="26.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="66.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="62.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.7109375" style="2"/>
-    <col min="6" max="16384" width="26.7109375" style="2" collapsed="1"/>
+    <col min="1" max="1" width="13.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="66.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="62.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.6640625" style="1"/>
+    <col min="6" max="16384" width="26.6640625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:30" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+    </row>
+    <row r="2" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>6</v>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{D31718E4-BE40-44FA-B6EF-77B1BB299B48}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{F91DD1C7-7912-4E17-A8F8-770BC9FA38BA}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -963,17 +1062,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>6</v>
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>